<commit_message>
create, get, delete subject, get list require
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HK6\schedule_API\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB77AA0-03E4-44A2-A101-79C1EA55B7BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326BE257-90AF-49FF-8BB6-7E6C3C84B9C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6504" yWindow="1872" windowWidth="17280" windowHeight="12348" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1764" yWindow="612" windowWidth="17280" windowHeight="12348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="require_subject" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
   <si>
     <t>type</t>
   </si>
@@ -42,18 +42,12 @@
     <t>description</t>
   </si>
   <si>
-    <t>Không học vào buổi chiều</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
     <t>grade</t>
   </si>
   <si>
-    <t>nLession</t>
-  </si>
-  <si>
     <t>Toán</t>
   </si>
   <si>
@@ -72,12 +66,6 @@
     <t>Ngoại ngữ</t>
   </si>
   <si>
-    <t>Không học qua giờ ra chơi</t>
-  </si>
-  <si>
-    <t>Không học vào thứ 2</t>
-  </si>
-  <si>
     <t>Giáo dục thể chất</t>
   </si>
   <si>
@@ -121,16 +109,55 @@
   </si>
   <si>
     <t>GDKT&amp;PL</t>
+  </si>
+  <si>
+    <t>nLesson</t>
+  </si>
+  <si>
+    <t>Ràng buộc 1</t>
+  </si>
+  <si>
+    <t>Ràng buộc 2</t>
+  </si>
+  <si>
+    <t>Ràng buộc 3</t>
+  </si>
+  <si>
+    <t>Ràng buộc 4</t>
+  </si>
+  <si>
+    <t>Ràng buộc 5</t>
+  </si>
+  <si>
+    <t>Ràng buộc 6</t>
+  </si>
+  <si>
+    <t>Ràng buộc 7</t>
+  </si>
+  <si>
+    <t>Ràng buộc 8</t>
+  </si>
+  <si>
+    <t>Ràng buộc 9</t>
+  </si>
+  <si>
+    <t>Ràng buộc 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -438,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -459,29 +486,86 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -490,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66602AFC-04EC-4B67-B335-B8FDD0216F89}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -504,24 +588,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -532,10 +616,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -546,10 +630,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -560,10 +644,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -574,10 +658,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -588,10 +672,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -602,10 +686,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -616,10 +700,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -630,10 +714,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -644,10 +728,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -658,10 +742,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -672,10 +756,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -686,10 +770,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -700,10 +784,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -714,10 +798,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -728,10 +812,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -742,10 +826,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>11</v>
@@ -756,10 +840,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>11</v>
@@ -770,10 +854,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C20">
         <v>11</v>
@@ -784,10 +868,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C21">
         <v>11</v>
@@ -798,10 +882,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>11</v>
@@ -812,10 +896,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C23">
         <v>11</v>
@@ -826,10 +910,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>11</v>
@@ -840,10 +924,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C25">
         <v>11</v>
@@ -854,10 +938,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C26">
         <v>11</v>
@@ -868,10 +952,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C27">
         <v>11</v>
@@ -882,10 +966,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C28">
         <v>11</v>
@@ -896,10 +980,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -910,10 +994,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -924,10 +1008,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C31">
         <v>11</v>
@@ -938,10 +1022,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C32">
         <v>11</v>
@@ -952,10 +1036,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C33">
         <v>11</v>
@@ -966,10 +1050,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C34">
         <v>12</v>
@@ -980,10 +1064,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C35">
         <v>12</v>
@@ -994,10 +1078,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C36">
         <v>12</v>
@@ -1008,10 +1092,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>12</v>
@@ -1022,10 +1106,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C38">
         <v>12</v>
@@ -1036,10 +1120,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C39">
         <v>12</v>
@@ -1050,10 +1134,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C40">
         <v>12</v>
@@ -1064,10 +1148,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C41">
         <v>12</v>
@@ -1078,10 +1162,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C42">
         <v>12</v>
@@ -1092,10 +1176,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C43">
         <v>12</v>
@@ -1106,10 +1190,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C44">
         <v>12</v>
@@ -1120,10 +1204,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C45">
         <v>12</v>
@@ -1134,10 +1218,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C46">
         <v>12</v>
@@ -1148,10 +1232,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C47">
         <v>12</v>
@@ -1162,10 +1246,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C48">
         <v>12</v>
@@ -1176,10 +1260,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C49">
         <v>12</v>

</xml_diff>

<commit_message>
get require teacher, update, delete teacher
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HK6\schedule_API\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326BE257-90AF-49FF-8BB6-7E6C3C84B9C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4391A3-ED6B-497D-B3AE-0EB7A2997FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1764" yWindow="612" windowWidth="17280" windowHeight="12348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="require_subject" sheetId="1" r:id="rId1"/>
-    <sheet name="suggest" sheetId="2" r:id="rId2"/>
+    <sheet name="require_teacher" sheetId="3" r:id="rId2"/>
+    <sheet name="suggest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="36">
   <si>
     <t>type</t>
   </si>
@@ -467,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -571,6 +572,112 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76537E0-B62C-4DD3-B848-262F0AFD0461}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66602AFC-04EC-4B67-B335-B8FDD0216F89}">
   <dimension ref="A1:D49"/>
   <sheetViews>

</xml_diff>

<commit_message>
generate scheduling school ver_1
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HK6\schedule_API\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4391A3-ED6B-497D-B3AE-0EB7A2997FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0663F5-9056-45C4-9A4B-0225DAA5598B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="require_subject" sheetId="1" r:id="rId1"/>
     <sheet name="require_teacher" sheetId="3" r:id="rId2"/>
     <sheet name="suggest" sheetId="2" r:id="rId3"/>
+    <sheet name="teacher" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="159">
   <si>
     <t>type</t>
   </si>
@@ -143,13 +144,382 @@
   </si>
   <si>
     <t>Ràng buộc 0</t>
+  </si>
+  <si>
+    <t>teacher_id</t>
+  </si>
+  <si>
+    <t>period_per_week</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>Trịnh Xuân Hoàng</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Toản</t>
+  </si>
+  <si>
+    <t>Dương Tùng Lâm</t>
+  </si>
+  <si>
+    <t>Phạm Đình Long</t>
+  </si>
+  <si>
+    <t>Quan Văn Chuẩn</t>
+  </si>
+  <si>
+    <t>Bùi Hoàng Việt Anh</t>
+  </si>
+  <si>
+    <t>Đặng Văn Tới</t>
+  </si>
+  <si>
+    <t>Lê Văn Xuân</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoàng Duy</t>
+  </si>
+  <si>
+    <t>Nguyễn Cảnh Anh</t>
+  </si>
+  <si>
+    <t>Âu Dương Quân</t>
+  </si>
+  <si>
+    <t>Dụng Quang Nho</t>
+  </si>
+  <si>
+    <t>Thái Bá Sang</t>
+  </si>
+  <si>
+    <t>Mai Sỹ Hoàng</t>
+  </si>
+  <si>
+    <t>Cao Trần Hoàng Hùng</t>
+  </si>
+  <si>
+    <t>Lê Thành Lâm</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Trọng</t>
+  </si>
+  <si>
+    <t>Trần Ngọc Hiệp</t>
+  </si>
+  <si>
+    <t>Nguyễn Cao Kỳ</t>
+  </si>
+  <si>
+    <t>Tiêu Exal</t>
+  </si>
+  <si>
+    <t>Nguyễn Duy Thắng</t>
+  </si>
+  <si>
+    <t>Đoàn Thanh Trường</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Minh</t>
+  </si>
+  <si>
+    <t>Trần Văn Công</t>
+  </si>
+  <si>
+    <t>Lý Công Hoàng Anh</t>
+  </si>
+  <si>
+    <t>Trần Bảo Toàn</t>
+  </si>
+  <si>
+    <t>Đặng Văn Lắm</t>
+  </si>
+  <si>
+    <t>Trần Ngọc Ánh</t>
+  </si>
+  <si>
+    <t>Hoàng Văn Hải</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoàng Bảo</t>
+  </si>
+  <si>
+    <t>Uông Ngọc Tiến</t>
+  </si>
+  <si>
+    <t>Nguyễn Trọng Long</t>
+  </si>
+  <si>
+    <t>Phạm Văn Luân</t>
+  </si>
+  <si>
+    <t>Võ Văn Toàn</t>
+  </si>
+  <si>
+    <t>Nguyễn Hồng Sơn</t>
+  </si>
+  <si>
+    <t>Nguyễn Hai Long</t>
+  </si>
+  <si>
+    <t>Trương Tiến Anh</t>
+  </si>
+  <si>
+    <t>Nguyễn Hữu Thắng</t>
+  </si>
+  <si>
+    <t>Nguyễn Thành Nhân</t>
+  </si>
+  <si>
+    <t>Mai Xuân Quyết</t>
+  </si>
+  <si>
+    <t>Hồ Thanh Minh</t>
+  </si>
+  <si>
+    <t>Nguyễn Trần Việt Cường</t>
+  </si>
+  <si>
+    <t>Trần Danh Trung</t>
+  </si>
+  <si>
+    <t>Nhâm Mạnh Dũng</t>
+  </si>
+  <si>
+    <t>Lê Minh Bình</t>
+  </si>
+  <si>
+    <t>Ngô Hoàng Anh</t>
+  </si>
+  <si>
+    <t>Lê Văn Nam</t>
+  </si>
+  <si>
+    <t>Huỳnh Tiến Đạt</t>
+  </si>
+  <si>
+    <t>Exal</t>
+  </si>
+  <si>
+    <t>C. Anh</t>
+  </si>
+  <si>
+    <t>T. Anh</t>
+  </si>
+  <si>
+    <t>H. Anh</t>
+  </si>
+  <si>
+    <t>Ánh</t>
+  </si>
+  <si>
+    <t>Bảo</t>
+  </si>
+  <si>
+    <t>Bình</t>
+  </si>
+  <si>
+    <t>Chuẩn</t>
+  </si>
+  <si>
+    <t>Công</t>
+  </si>
+  <si>
+    <t>Đạt</t>
+  </si>
+  <si>
+    <t>Dũng</t>
+  </si>
+  <si>
+    <t>Duy</t>
+  </si>
+  <si>
+    <t>Hải</t>
+  </si>
+  <si>
+    <t>Hiệp</t>
+  </si>
+  <si>
+    <t>Kỳ</t>
+  </si>
+  <si>
+    <t>Lắm</t>
+  </si>
+  <si>
+    <t>Hoàng Anh</t>
+  </si>
+  <si>
+    <t>Hoàng Hùng</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Nhân</t>
+  </si>
+  <si>
+    <t>Nho</t>
+  </si>
+  <si>
+    <t>Quân</t>
+  </si>
+  <si>
+    <t>Quyết</t>
+  </si>
+  <si>
+    <t>Sang</t>
+  </si>
+  <si>
+    <t>Sơn</t>
+  </si>
+  <si>
+    <t>Tiến</t>
+  </si>
+  <si>
+    <t>Toản</t>
+  </si>
+  <si>
+    <t>Tới</t>
+  </si>
+  <si>
+    <t>Trọng</t>
+  </si>
+  <si>
+    <t>Trung</t>
+  </si>
+  <si>
+    <t>Trường</t>
+  </si>
+  <si>
+    <t>Việt Anh</t>
+  </si>
+  <si>
+    <t>Việt Cường</t>
+  </si>
+  <si>
+    <t>Xuân</t>
+  </si>
+  <si>
+    <t>X. Hoàng</t>
+  </si>
+  <si>
+    <t>S. Hoàng</t>
+  </si>
+  <si>
+    <t>Thành Lâm</t>
+  </si>
+  <si>
+    <t>Tùng Lâm</t>
+  </si>
+  <si>
+    <t>Đình Long</t>
+  </si>
+  <si>
+    <t>Trọng Long</t>
+  </si>
+  <si>
+    <t>Hai Long</t>
+  </si>
+  <si>
+    <t>Văn Minh</t>
+  </si>
+  <si>
+    <t>Thanh Minh</t>
+  </si>
+  <si>
+    <t>Duy Thắng</t>
+  </si>
+  <si>
+    <t>Hữu Thắng</t>
+  </si>
+  <si>
+    <t>Bảo Toàn</t>
+  </si>
+  <si>
+    <t>Văn Toàn</t>
+  </si>
+  <si>
+    <t>Đinh Văn Ngọc</t>
+  </si>
+  <si>
+    <t>Phạm Đình Luân</t>
+  </si>
+  <si>
+    <t>Phạm Bá Minh</t>
+  </si>
+  <si>
+    <t>Lê Chí Nhin</t>
+  </si>
+  <si>
+    <t>Nguyễn Duy Huy</t>
+  </si>
+  <si>
+    <t>Lý Thiên Ân</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Cẩm Nhung</t>
+  </si>
+  <si>
+    <t>Phạm Hoàng Mẫn</t>
+  </si>
+  <si>
+    <t>Trần Văn Cương</t>
+  </si>
+  <si>
+    <t>Lã Chí Cường</t>
+  </si>
+  <si>
+    <t>Tạ Hoàng Hạc</t>
+  </si>
+  <si>
+    <t>Lê Kha Vĩ</t>
+  </si>
+  <si>
+    <t>Ngọc</t>
+  </si>
+  <si>
+    <t>Huy</t>
+  </si>
+  <si>
+    <t>Ân</t>
+  </si>
+  <si>
+    <t>Nhung</t>
+  </si>
+  <si>
+    <t>Mẫn</t>
+  </si>
+  <si>
+    <t>Cương</t>
+  </si>
+  <si>
+    <t>Cường</t>
+  </si>
+  <si>
+    <t>Hạc</t>
+  </si>
+  <si>
+    <t>Vĩ</t>
+  </si>
+  <si>
+    <t>Bá Minh</t>
+  </si>
+  <si>
+    <t>Chí Nhin</t>
+  </si>
+  <si>
+    <t>Văn Luân</t>
+  </si>
+  <si>
+    <t>Đình Luân</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,16 +533,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -180,12 +563,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.59999389629810485"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="0.59999389629810485"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="0.59999389629810485"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.59999389629810485"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76537E0-B62C-4DD3-B848-262F0AFD0461}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -681,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66602AFC-04EC-4B67-B335-B8FDD0216F89}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1382,4 +1786,1068 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF4D05C-10B6-47AC-A6C3-DB1B3E5119BD}">
+  <dimension ref="A1:E61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.3984375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.8984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.09765625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.796875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.59765625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.796875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="4">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="4">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="4">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="4">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="4">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="4">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="4">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="4">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="4">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" s="4">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="4">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="4">
+        <v>10</v>
+      </c>
+      <c r="D15" s="4">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="4">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="4">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="4">
+        <v>10</v>
+      </c>
+      <c r="D18" s="4">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="4">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="4">
+        <v>10</v>
+      </c>
+      <c r="D20" s="4">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="4">
+        <v>10</v>
+      </c>
+      <c r="D21" s="4">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="4">
+        <v>10</v>
+      </c>
+      <c r="D22" s="4">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="4">
+        <v>10</v>
+      </c>
+      <c r="D23" s="4">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="4">
+        <v>10</v>
+      </c>
+      <c r="D24" s="4">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="4">
+        <v>10</v>
+      </c>
+      <c r="D25" s="4">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="4">
+        <v>10</v>
+      </c>
+      <c r="D26" s="4">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C27" s="4">
+        <v>10</v>
+      </c>
+      <c r="D27" s="4">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="4">
+        <v>10</v>
+      </c>
+      <c r="D28" s="4">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" s="4">
+        <v>10</v>
+      </c>
+      <c r="D29" s="4">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="4">
+        <v>10</v>
+      </c>
+      <c r="D30" s="4">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="4">
+        <v>10</v>
+      </c>
+      <c r="D31" s="4">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="4">
+        <v>10</v>
+      </c>
+      <c r="D32" s="4">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33" s="4">
+        <v>10</v>
+      </c>
+      <c r="D33" s="4">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="4">
+        <v>10</v>
+      </c>
+      <c r="D34" s="4">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="4">
+        <v>10</v>
+      </c>
+      <c r="D35" s="4">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="4">
+        <v>10</v>
+      </c>
+      <c r="D36" s="4">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="4">
+        <v>10</v>
+      </c>
+      <c r="D37" s="4">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C38" s="4">
+        <v>10</v>
+      </c>
+      <c r="D38" s="4">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="4">
+        <v>10</v>
+      </c>
+      <c r="D39" s="4">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="4">
+        <v>10</v>
+      </c>
+      <c r="D40" s="4">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" s="4">
+        <v>10</v>
+      </c>
+      <c r="D41" s="4">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="4">
+        <v>10</v>
+      </c>
+      <c r="D42" s="4">
+        <v>11</v>
+      </c>
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="4">
+        <v>10</v>
+      </c>
+      <c r="D43" s="4">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="4">
+        <v>10</v>
+      </c>
+      <c r="D44" s="4">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" s="4">
+        <v>10</v>
+      </c>
+      <c r="D45" s="4">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="4">
+        <v>10</v>
+      </c>
+      <c r="D46" s="4">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="4">
+        <v>10</v>
+      </c>
+      <c r="D47" s="4">
+        <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="4">
+        <v>10</v>
+      </c>
+      <c r="D48" s="4">
+        <v>12</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="4">
+        <v>10</v>
+      </c>
+      <c r="D49" s="4">
+        <v>12</v>
+      </c>
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="4">
+        <v>10</v>
+      </c>
+      <c r="D50" s="4">
+        <v>12</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="4">
+        <v>10</v>
+      </c>
+      <c r="D51" s="4">
+        <v>11</v>
+      </c>
+      <c r="E51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C52" s="4">
+        <v>10</v>
+      </c>
+      <c r="D52" s="4">
+        <v>12</v>
+      </c>
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="4">
+        <v>10</v>
+      </c>
+      <c r="D53" s="4">
+        <v>12</v>
+      </c>
+      <c r="E53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" s="4">
+        <v>10</v>
+      </c>
+      <c r="D54" s="4">
+        <v>10</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C55" s="4">
+        <v>10</v>
+      </c>
+      <c r="D55" s="4">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C56" s="4">
+        <v>10</v>
+      </c>
+      <c r="D56" s="4">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" s="4">
+        <v>10</v>
+      </c>
+      <c r="D57" s="4">
+        <v>12</v>
+      </c>
+      <c r="E57" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="4">
+        <v>10</v>
+      </c>
+      <c r="D58" s="4">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" s="4">
+        <v>10</v>
+      </c>
+      <c r="D59" s="4">
+        <v>12</v>
+      </c>
+      <c r="E59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="4">
+        <v>10</v>
+      </c>
+      <c r="D60" s="4">
+        <v>10</v>
+      </c>
+      <c r="E60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" s="4">
+        <v>10</v>
+      </c>
+      <c r="D61" s="4">
+        <v>12</v>
+      </c>
+      <c r="E61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E61">
+    <sortCondition ref="B1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
generate scheduling school v_2
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HK6\schedule_API\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0663F5-9056-45C4-9A4B-0225DAA5598B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93ABB1AF-F2F4-4DC1-997B-06B76710CEF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="require_subject" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="156">
   <si>
     <t>type</t>
   </si>
@@ -93,15 +93,6 @@
   </si>
   <si>
     <t>sortName</t>
-  </si>
-  <si>
-    <t>Chào cờ</t>
-  </si>
-  <si>
-    <t>Sinh hoạt chủ nhiệm</t>
-  </si>
-  <si>
-    <t>SHCN</t>
   </si>
   <si>
     <t>GDTC</t>
@@ -894,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -902,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -910,7 +901,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -918,7 +909,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -926,7 +917,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -934,7 +925,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -942,7 +933,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -950,7 +941,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -958,7 +949,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -966,7 +957,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +992,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1009,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1017,7 +1008,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1025,7 +1016,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1033,7 +1024,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1041,7 +1032,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1049,7 +1040,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1057,7 +1048,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1065,7 +1056,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1073,7 +1064,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1083,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66602AFC-04EC-4B67-B335-B8FDD0216F89}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1108,43 +1099,43 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -1155,66 +1146,66 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -1225,38 +1216,38 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -1267,24 +1258,24 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>10</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>10</v>
@@ -1295,10 +1286,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -1309,122 +1300,122 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>11</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>11</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>11</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>11</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C22">
         <v>11</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C23">
         <v>11</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>11</v>
@@ -1435,38 +1426,38 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C25">
         <v>11</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C26">
         <v>11</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C27">
         <v>11</v>
@@ -1477,10 +1468,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C28">
         <v>11</v>
@@ -1491,91 +1482,91 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C29">
         <v>11</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C32">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C33">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C34">
         <v>12</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B35" t="s">
         <v>21</v>
@@ -1589,52 +1580,52 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C36">
         <v>12</v>
       </c>
       <c r="D36">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C37">
         <v>12</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C38">
         <v>12</v>
       </c>
       <c r="D38">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C39">
         <v>12</v>
@@ -1645,10 +1636,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C40">
         <v>12</v>
@@ -1659,10 +1650,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C41">
         <v>12</v>
@@ -1673,113 +1664,29 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C42">
         <v>12</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C43">
         <v>12</v>
       </c>
       <c r="D43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44">
-        <v>12</v>
-      </c>
-      <c r="D44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45">
-        <v>12</v>
-      </c>
-      <c r="D45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46">
-        <v>12</v>
-      </c>
-      <c r="D46">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47">
-        <v>12</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48">
-        <v>12</v>
-      </c>
-      <c r="D48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>17</v>
-      </c>
-      <c r="B49" t="s">
-        <v>17</v>
-      </c>
-      <c r="C49">
-        <v>12</v>
-      </c>
-      <c r="D49">
         <v>1</v>
       </c>
     </row>
@@ -1792,7 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAF4D05C-10B6-47AC-A6C3-DB1B3E5119BD}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1811,24 +1718,24 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C2" s="4">
         <v>10</v>
@@ -1842,10 +1749,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C3" s="4">
         <v>10</v>
@@ -1859,10 +1766,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C4" s="4">
         <v>10</v>
@@ -1871,15 +1778,15 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C5" s="4">
         <v>10</v>
@@ -1893,10 +1800,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C6" s="4">
         <v>10</v>
@@ -1910,10 +1817,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C7" s="4">
         <v>10</v>
@@ -1927,10 +1834,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C8" s="4">
         <v>10</v>
@@ -1944,10 +1851,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C9" s="4">
         <v>10</v>
@@ -1956,15 +1863,15 @@
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C10" s="4">
         <v>10</v>
@@ -1978,10 +1885,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C11" s="4">
         <v>10</v>
@@ -1995,10 +1902,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C12" s="4">
         <v>10</v>
@@ -2012,10 +1919,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C13" s="4">
         <v>10</v>
@@ -2029,10 +1936,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C14" s="4">
         <v>10</v>
@@ -2046,10 +1953,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C15" s="4">
         <v>10</v>
@@ -2063,10 +1970,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C16" s="4">
         <v>10</v>
@@ -2075,15 +1982,15 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C17" s="4">
         <v>10</v>
@@ -2092,15 +1999,15 @@
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C18" s="4">
         <v>10</v>
@@ -2114,10 +2021,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C19" s="4">
         <v>10</v>
@@ -2126,15 +2033,15 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C20" s="4">
         <v>10</v>
@@ -2148,10 +2055,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C21" s="4">
         <v>10</v>
@@ -2165,10 +2072,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C22" s="4">
         <v>10</v>
@@ -2182,10 +2089,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C23" s="4">
         <v>10</v>
@@ -2199,10 +2106,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C24" s="4">
         <v>10</v>
@@ -2216,10 +2123,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C25" s="4">
         <v>10</v>
@@ -2233,10 +2140,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C26" s="4">
         <v>10</v>
@@ -2250,10 +2157,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C27" s="4">
         <v>10</v>
@@ -2267,10 +2174,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C28" s="4">
         <v>10</v>
@@ -2284,10 +2191,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C29" s="4">
         <v>10</v>
@@ -2301,10 +2208,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C30" s="4">
         <v>10</v>
@@ -2318,10 +2225,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C31" s="4">
         <v>10</v>
@@ -2335,10 +2242,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C32" s="4">
         <v>10</v>
@@ -2347,15 +2254,15 @@
         <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C33" s="4">
         <v>10</v>
@@ -2369,10 +2276,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C34" s="4">
         <v>10</v>
@@ -2386,10 +2293,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C35" s="4">
         <v>10</v>
@@ -2403,10 +2310,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C36" s="4">
         <v>10</v>
@@ -2415,15 +2322,15 @@
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C37" s="4">
         <v>10</v>
@@ -2432,15 +2339,15 @@
         <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C38" s="4">
         <v>10</v>
@@ -2454,10 +2361,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C39" s="4">
         <v>10</v>
@@ -2466,15 +2373,15 @@
         <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C40" s="4">
         <v>10</v>
@@ -2488,10 +2395,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C41" s="4">
         <v>10</v>
@@ -2505,10 +2412,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C42" s="4">
         <v>10</v>
@@ -2522,10 +2429,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C43" s="4">
         <v>10</v>
@@ -2539,10 +2446,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C44" s="4">
         <v>10</v>
@@ -2556,10 +2463,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C45" s="4">
         <v>10</v>
@@ -2573,10 +2480,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C46" s="4">
         <v>10</v>
@@ -2590,10 +2497,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C47" s="4">
         <v>10</v>
@@ -2607,10 +2514,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C48" s="4">
         <v>10</v>
@@ -2624,10 +2531,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C49" s="4">
         <v>10</v>
@@ -2641,10 +2548,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C50" s="4">
         <v>10</v>
@@ -2658,10 +2565,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C51" s="4">
         <v>10</v>
@@ -2675,10 +2582,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C52" s="4">
         <v>10</v>
@@ -2692,10 +2599,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C53" s="4">
         <v>10</v>
@@ -2709,10 +2616,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C54" s="4">
         <v>10</v>
@@ -2726,10 +2633,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C55" s="4">
         <v>10</v>
@@ -2743,10 +2650,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C56" s="4">
         <v>10</v>
@@ -2760,10 +2667,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C57" s="4">
         <v>10</v>
@@ -2777,10 +2684,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C58" s="4">
         <v>10</v>
@@ -2794,10 +2701,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C59" s="4">
         <v>10</v>
@@ -2811,10 +2718,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C60" s="4">
         <v>10</v>
@@ -2828,10 +2735,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C61" s="4">
         <v>10</v>

</xml_diff>